<commit_message>
move class course to lms file
</commit_message>
<xml_diff>
--- a/session/import/12775191 - check lịch lặp.xlsx
+++ b/session/import/12775191 - check lịch lặp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cadca85d68a966ba/LMS/session/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_DED00142D7A7720244CF6F5534CD029800E0B574" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5215D0A1-4F0D-43CD-A0EA-9347A43ED5D4}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_DED00142245F330734CE6F55340A6A5D2DFEB7C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{781CAD64-9393-224D-9CFC-C05D2038F0D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>GHI CHÚ:
 1. Dữ liệu điểm danh: điền 1 là Có mặt, điền 0 là Vắng mặt, để trống là không nhập
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>check lịch lặp 1 (T4, 29.11.23)</t>
+  </si>
+  <si>
+    <t>check lịch lặp 1 (T5, 30.11.23)</t>
   </si>
   <si>
     <t>admindv1</t>
@@ -117,11 +120,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -454,19 +459,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,7 +480,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,112 +505,115 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>

</xml_diff>

<commit_message>
fix pass_master: move arg type_school to index 3
</commit_message>
<xml_diff>
--- a/session/import/12775191 - check lịch lặp.xlsx
+++ b/session/import/12775191 - check lịch lặp.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cadca85d68a966ba/LMS/session/import/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_DED00142245F330734CE6F55340A6A5D2DFEB7C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{781CAD64-9393-224D-9CFC-C05D2038F0D2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>GHI CHÚ:
 1. Dữ liệu điểm danh: điền 1 là Có mặt, điền 0 là Vắng mặt, để trống là không nhập
@@ -108,25 +103,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,41 +139,34 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -458,20 +456,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="30.7109375" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="true" style="0"/>
+    <col min="2" max="2" width="32.42578125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" customHeight="1" ht="57.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +481,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,122 +510,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="1">
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>